<commit_message>
excel file bug fixed
</commit_message>
<xml_diff>
--- a/attendance/Oct-31-2022.xlsx
+++ b/attendance/Oct-31-2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -31,19 +31,22 @@
     <t>In Time</t>
   </si>
   <si>
-    <t>chanchal</t>
-  </si>
-  <si>
-    <t>AIML-B</t>
+    <t>S190933435</t>
+  </si>
+  <si>
+    <t>CSE-D</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>01:19 PM</t>
+    <t>11:15 PM</t>
+  </si>
+  <si>
+    <t>S190933433</t>
+  </si>
+  <si>
+    <t>suyog</t>
   </si>
 </sst>
 </file>
@@ -375,7 +378,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -409,10 +412,44 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
         <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>